<commit_message>
published state of ETdataset on 1st of August 2019
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/energy/energy_chp_ultra_supercritical_coal.central_producer.xlsx
+++ b/nodes_source_analyses/energy/energy_chp_ultra_supercritical_coal.central_producer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marliekeverweij/Projects/etdataset/nodes_source_analyses/energy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michieldenhaan/Projects/etdataset/nodes_source_analyses/energy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B1E2D2-DBF4-8745-AE93-4B14F3FAE80B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8ACF49-22DC-9A4F-BDE8-B008F7959E57}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="460" windowWidth="25600" windowHeight="15900" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,10 +37,16 @@
     <definedName name="Wp_to_kWp">#REF!</definedName>
     <definedName name="WP_to_MWp">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -239,9 +245,6 @@
   </si>
   <si>
     <t>input.coal</t>
-  </si>
-  <si>
-    <t>input.torrified_biomass_pellets</t>
   </si>
   <si>
     <t>euro/FLH</t>
@@ -830,6 +833,9 @@
   <si>
     <t xml:space="preserve">This sheet summarizes all node attributes formatted in the way they are used by the Energy Transition Model. Use the Excel formulas to find the original data and sources for these numbers. You can also use this document to update the attribute value. Once you have finished updating, save this document and run rake import:node NODE="nodename" to update the node attributes on ETSource. 
 </t>
+  </si>
+  <si>
+    <t>input.torrefied_biomass_pellets</t>
   </si>
 </sst>
 </file>
@@ -963,6 +969,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -970,6 +977,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -977,6 +985,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -984,6 +993,7 @@
       <sz val="16"/>
       <color rgb="FF1F497D"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -991,17 +1001,20 @@
       <sz val="12"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1015,6 +1028,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2794,16 +2808,16 @@
         <v>20</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="7"/>
       <c r="B5" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>111</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2828,7 +2842,7 @@
     <row r="9" spans="1:3">
       <c r="A9" s="7"/>
       <c r="B9" s="111" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C9" s="112"/>
     </row>
@@ -2840,31 +2854,31 @@
     <row r="11" spans="1:3">
       <c r="A11" s="7"/>
       <c r="B11" s="113" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="115" t="s">
         <v>97</v>
-      </c>
-      <c r="C11" s="115" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" thickBot="1">
       <c r="A12" s="7"/>
       <c r="B12" s="113"/>
       <c r="C12" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" thickBot="1">
       <c r="A13" s="7"/>
       <c r="B13" s="113"/>
       <c r="C13" s="116" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="7"/>
       <c r="B14" s="113"/>
       <c r="C14" s="114" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2875,58 +2889,58 @@
     <row r="16" spans="1:3">
       <c r="A16" s="7"/>
       <c r="B16" s="113" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="117" t="s">
         <v>102</v>
-      </c>
-      <c r="C16" s="117" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="7"/>
       <c r="B17" s="113"/>
       <c r="C17" s="118" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="7"/>
       <c r="B18" s="113"/>
       <c r="C18" s="119" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="7"/>
       <c r="B19" s="113"/>
       <c r="C19" s="120" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="7"/>
       <c r="B20" s="121"/>
       <c r="C20" s="122" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="7"/>
       <c r="B21" s="121"/>
       <c r="C21" s="123" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="7"/>
       <c r="B22" s="121"/>
       <c r="C22" s="124" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="B23" s="121"/>
       <c r="C23" s="125" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2942,8 +2956,8 @@
   </sheetPr>
   <dimension ref="B1:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD24"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -2973,7 +2987,7 @@
     </row>
     <row r="2" spans="2:11">
       <c r="B2" s="172" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C2" s="173"/>
       <c r="D2" s="173"/>
@@ -3069,7 +3083,7 @@
     <row r="10" spans="2:11" s="5" customFormat="1" ht="19" thickBot="1">
       <c r="B10" s="37"/>
       <c r="C10" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D10" s="45"/>
       <c r="E10" s="23"/>
@@ -3094,7 +3108,7 @@
       <c r="G11" s="28"/>
       <c r="H11" s="44"/>
       <c r="I11" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J11" s="22"/>
     </row>
@@ -3113,7 +3127,7 @@
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
       <c r="I12" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J12" s="145"/>
       <c r="K12" s="3"/>
@@ -3133,7 +3147,7 @@
       <c r="G13" s="28"/>
       <c r="H13" s="28"/>
       <c r="I13" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J13" s="145"/>
       <c r="K13" s="3"/>
@@ -3153,7 +3167,7 @@
       <c r="G14" s="28"/>
       <c r="H14" s="28"/>
       <c r="I14" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J14" s="145"/>
       <c r="K14" s="3"/>
@@ -3173,7 +3187,7 @@
       <c r="G15" s="28"/>
       <c r="H15" s="28"/>
       <c r="I15" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J15" s="145"/>
       <c r="K15" s="3"/>
@@ -3193,7 +3207,7 @@
       <c r="G16" s="28"/>
       <c r="H16" s="28"/>
       <c r="I16" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J16" s="146"/>
       <c r="K16" s="1"/>
@@ -3213,7 +3227,7 @@
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>
       <c r="I17" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J17" s="146"/>
       <c r="K17" s="1"/>
@@ -3224,7 +3238,7 @@
         <v>47</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E18" s="53">
         <f>'Research data'!H6</f>
@@ -3236,7 +3250,7 @@
       </c>
       <c r="H18" s="28"/>
       <c r="I18" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J18" s="145"/>
     </row>
@@ -3246,18 +3260,18 @@
         <v>48</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E19" s="53">
         <v>260.86956521739103</v>
       </c>
       <c r="F19" s="28"/>
       <c r="G19" s="51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H19" s="28"/>
       <c r="I19" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J19" s="145"/>
     </row>
@@ -3275,7 +3289,7 @@
     <row r="21" spans="2:11" ht="17" thickBot="1">
       <c r="B21" s="32"/>
       <c r="C21" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D21" s="143"/>
       <c r="E21" s="136"/>
@@ -3303,7 +3317,7 @@
       </c>
       <c r="H22" s="28"/>
       <c r="I22" s="52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J22" s="147"/>
     </row>
@@ -3320,11 +3334,11 @@
       </c>
       <c r="F23" s="28"/>
       <c r="G23" s="51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H23" s="28"/>
       <c r="I23" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J23" s="147"/>
     </row>
@@ -3345,7 +3359,7 @@
       </c>
       <c r="H24" s="28"/>
       <c r="I24" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J24" s="145"/>
     </row>
@@ -3366,7 +3380,7 @@
       </c>
       <c r="H25" s="28"/>
       <c r="I25" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J25" s="145"/>
     </row>
@@ -3376,7 +3390,7 @@
         <v>52</v>
       </c>
       <c r="D26" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E26" s="135">
         <f>'Research data'!H16</f>
@@ -3384,11 +3398,11 @@
       </c>
       <c r="F26" s="28"/>
       <c r="G26" s="51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H26" s="28"/>
       <c r="I26" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J26" s="145"/>
     </row>
@@ -3398,7 +3412,7 @@
         <v>53</v>
       </c>
       <c r="D27" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E27" s="49">
         <f>'Research data'!H18</f>
@@ -3406,11 +3420,11 @@
       </c>
       <c r="F27" s="28"/>
       <c r="G27" s="51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H27" s="28"/>
       <c r="I27" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J27" s="145"/>
     </row>
@@ -3420,18 +3434,18 @@
         <v>54</v>
       </c>
       <c r="D28" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E28" s="49">
         <v>0</v>
       </c>
       <c r="F28" s="28"/>
       <c r="G28" s="51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H28" s="28"/>
       <c r="I28" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J28" s="145"/>
     </row>
@@ -3452,7 +3466,7 @@
       </c>
       <c r="H29" s="28"/>
       <c r="I29" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J29" s="145"/>
     </row>
@@ -3471,7 +3485,7 @@
       <c r="G30" s="28"/>
       <c r="H30" s="28"/>
       <c r="I30" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J30" s="145"/>
     </row>
@@ -3517,7 +3531,7 @@
       </c>
       <c r="H33" s="28"/>
       <c r="I33" s="52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J33" s="145"/>
     </row>
@@ -3539,7 +3553,7 @@
       </c>
       <c r="H34" s="28"/>
       <c r="I34" s="158" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J34" s="145"/>
     </row>
@@ -3561,7 +3575,7 @@
       </c>
       <c r="H35" s="28"/>
       <c r="I35" s="158" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J35" s="145"/>
     </row>
@@ -3580,7 +3594,7 @@
       <c r="G36" s="28"/>
       <c r="H36" s="28"/>
       <c r="I36" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J36" s="145"/>
     </row>
@@ -3599,7 +3613,7 @@
       <c r="G37" s="28"/>
       <c r="H37" s="28"/>
       <c r="I37" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J37" s="145"/>
     </row>
@@ -3618,7 +3632,7 @@
       <c r="G38" s="28"/>
       <c r="H38" s="28"/>
       <c r="I38" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J38" s="145"/>
     </row>
@@ -3637,7 +3651,7 @@
       <c r="G39" s="28"/>
       <c r="H39" s="28"/>
       <c r="I39" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J39" s="145"/>
     </row>
@@ -3656,7 +3670,7 @@
       <c r="G40" s="28"/>
       <c r="H40" s="28"/>
       <c r="I40" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J40" s="145"/>
     </row>
@@ -3675,7 +3689,7 @@
       <c r="G41" s="28"/>
       <c r="H41" s="28"/>
       <c r="I41" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J41" s="145"/>
     </row>
@@ -3694,14 +3708,14 @@
       <c r="G42" s="28"/>
       <c r="H42" s="28"/>
       <c r="I42" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J42" s="145"/>
     </row>
     <row r="43" spans="2:10" ht="17" thickBot="1">
       <c r="B43" s="32"/>
       <c r="C43" s="48" t="s">
-        <v>63</v>
+        <v>156</v>
       </c>
       <c r="D43" s="33" t="s">
         <v>5</v>
@@ -3713,7 +3727,7 @@
       <c r="G43" s="28"/>
       <c r="H43" s="28"/>
       <c r="I43" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J43" s="145"/>
     </row>
@@ -4011,7 +4025,7 @@
     <row r="3" spans="2:20" s="38" customFormat="1">
       <c r="B3" s="37"/>
       <c r="C3" s="130" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
@@ -4020,11 +4034,11 @@
       </c>
       <c r="G3" s="130"/>
       <c r="H3" s="130" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I3" s="130"/>
       <c r="J3" s="131" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K3" s="131"/>
       <c r="L3" s="131" t="s">
@@ -4032,19 +4046,19 @@
       </c>
       <c r="M3" s="131"/>
       <c r="N3" s="131" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O3" s="130"/>
       <c r="P3" s="131" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q3" s="131"/>
       <c r="R3" s="131" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="S3" s="130"/>
       <c r="T3" s="130" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="2:20">
@@ -4071,7 +4085,7 @@
     <row r="5" spans="2:20" ht="17" thickBot="1">
       <c r="B5" s="57"/>
       <c r="C5" s="46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D5" s="46"/>
       <c r="E5" s="46"/>
@@ -4099,7 +4113,7 @@
       <c r="D6" s="86"/>
       <c r="E6" s="86"/>
       <c r="F6" s="126" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G6" s="134"/>
       <c r="H6" s="88">
@@ -4187,7 +4201,7 @@
         <v>0.28313100000000002</v>
       </c>
       <c r="T9" s="138" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="2:20" ht="17" thickBot="1">
@@ -4222,7 +4236,7 @@
       <c r="Q10" s="84"/>
       <c r="R10" s="84"/>
       <c r="T10" s="50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="2:20" ht="17" thickBot="1">
@@ -4257,7 +4271,7 @@
       <c r="Q11" s="84"/>
       <c r="R11" s="84"/>
       <c r="T11" s="50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="2:20">
@@ -4283,7 +4297,7 @@
     <row r="13" spans="2:20" ht="17" thickBot="1">
       <c r="B13" s="57"/>
       <c r="C13" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
@@ -4305,7 +4319,7 @@
     <row r="14" spans="2:20" ht="17" thickBot="1">
       <c r="B14" s="57"/>
       <c r="C14" s="137" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="21"/>
@@ -4328,18 +4342,18 @@
       <c r="Q14" s="97"/>
       <c r="R14" s="97"/>
       <c r="T14" s="149" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="2:20" ht="17" thickBot="1">
       <c r="B15" s="57"/>
       <c r="C15" s="137" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D15" s="103"/>
       <c r="E15" s="103"/>
       <c r="F15" s="126" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G15" s="134"/>
       <c r="H15" s="102">
@@ -4359,18 +4373,18 @@
       <c r="Q15" s="97"/>
       <c r="R15" s="97"/>
       <c r="T15" s="170" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="2:20" ht="17" thickBot="1">
       <c r="B16" s="57"/>
       <c r="C16" s="137" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D16" s="46"/>
       <c r="E16" s="46"/>
       <c r="F16" s="128" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G16" s="128"/>
       <c r="H16" s="105">
@@ -4388,18 +4402,18 @@
       <c r="Q16" s="94"/>
       <c r="R16" s="94"/>
       <c r="T16" s="149" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="2:20" ht="17" thickBot="1">
       <c r="B17" s="57"/>
       <c r="C17" s="137" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D17" s="46"/>
       <c r="E17" s="46"/>
       <c r="F17" s="128" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G17" s="128"/>
       <c r="H17" s="105">
@@ -4416,18 +4430,18 @@
       <c r="Q17" s="94"/>
       <c r="R17" s="94"/>
       <c r="T17" s="50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="2:20" ht="17" thickBot="1">
       <c r="B18" s="57"/>
       <c r="C18" s="137" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D18" s="107"/>
       <c r="E18" s="107"/>
       <c r="F18" s="87" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G18" s="89"/>
       <c r="H18" s="102">
@@ -4445,18 +4459,18 @@
       <c r="Q18" s="94"/>
       <c r="R18" s="94"/>
       <c r="T18" s="129" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="2:20" ht="17" thickBot="1">
       <c r="B19" s="57"/>
       <c r="C19" s="137" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D19" s="106"/>
       <c r="E19" s="106"/>
       <c r="F19" s="87" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G19" s="89"/>
       <c r="H19" s="102">
@@ -4474,18 +4488,18 @@
       <c r="Q19" s="94"/>
       <c r="R19" s="94"/>
       <c r="T19" s="50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="2:20" ht="17" thickBot="1">
       <c r="B20" s="57"/>
       <c r="C20" s="137" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D20" s="106"/>
       <c r="E20" s="106"/>
       <c r="F20" s="126" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G20" s="134"/>
       <c r="H20" s="102">
@@ -4506,12 +4520,12 @@
     <row r="21" spans="2:20" ht="17" thickBot="1">
       <c r="B21" s="57"/>
       <c r="C21" s="137" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D21" s="85"/>
       <c r="E21" s="85"/>
       <c r="F21" s="85" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G21" s="58"/>
       <c r="H21" s="108">
@@ -4532,12 +4546,12 @@
     <row r="22" spans="2:20" ht="17" thickBot="1">
       <c r="B22" s="57"/>
       <c r="C22" s="148" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D22" s="85"/>
       <c r="E22" s="85"/>
       <c r="F22" s="129" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G22" s="114"/>
       <c r="H22" s="108">
@@ -4653,13 +4667,13 @@
         <v>35</v>
       </c>
       <c r="G5" s="70" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H5" s="70" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I5" s="71" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J5" s="70" t="s">
         <v>18</v>
@@ -4676,7 +4690,7 @@
       <c r="I6" s="66"/>
       <c r="J6" s="65"/>
     </row>
-    <row r="7" spans="2:10" ht="32">
+    <row r="7" spans="2:10" ht="34">
       <c r="B7" s="64"/>
       <c r="C7" s="72"/>
       <c r="D7" s="72" t="s">
@@ -4686,17 +4700,17 @@
         <v>25</v>
       </c>
       <c r="F7" s="77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G7" s="150">
         <v>2010</v>
       </c>
       <c r="H7" s="77"/>
       <c r="I7" s="78" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J7" s="79" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="2:10">
@@ -4736,33 +4750,33 @@
       <c r="I10" s="78"/>
       <c r="J10" s="72"/>
     </row>
-    <row r="11" spans="2:10" s="151" customFormat="1" ht="32">
+    <row r="11" spans="2:10" s="151" customFormat="1" ht="34">
       <c r="B11" s="154"/>
       <c r="C11" s="160"/>
       <c r="D11" s="161" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E11" s="162" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F11" s="163" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G11" s="164" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H11" s="163"/>
       <c r="I11" s="171" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J11" s="161" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="2:10" s="151" customFormat="1">
       <c r="B12" s="154"/>
       <c r="C12" s="165" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D12" s="161"/>
       <c r="E12" s="155"/>
@@ -4775,7 +4789,7 @@
     <row r="13" spans="2:10" s="151" customFormat="1">
       <c r="B13" s="154"/>
       <c r="C13" s="165" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D13" s="161"/>
       <c r="E13" s="155"/>
@@ -4800,27 +4814,27 @@
       <c r="B15" s="64"/>
       <c r="C15" s="72"/>
       <c r="D15" s="72" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E15" s="67" t="s">
         <v>10</v>
       </c>
       <c r="F15" s="68" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G15" s="68" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H15" s="68"/>
       <c r="I15" s="68" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J15" s="79"/>
     </row>
     <row r="16" spans="2:10">
       <c r="B16" s="64"/>
       <c r="C16" s="75" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D16" s="72"/>
       <c r="E16" s="67"/>
@@ -4845,25 +4859,25 @@
       <c r="B18" s="64"/>
       <c r="C18" s="72"/>
       <c r="D18" s="72" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E18" s="67"/>
       <c r="F18" s="68">
         <v>2013</v>
       </c>
       <c r="G18" s="68" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H18" s="68"/>
       <c r="I18" s="68"/>
       <c r="J18" s="79" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="2:10">
       <c r="B19" s="64"/>
       <c r="C19" s="72" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D19" s="72"/>
       <c r="E19" s="67"/>
@@ -4876,7 +4890,7 @@
     <row r="20" spans="2:10">
       <c r="B20" s="64"/>
       <c r="C20" s="75" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D20" s="72"/>
       <c r="E20" s="67"/>
@@ -4889,7 +4903,7 @@
     <row r="21" spans="2:10">
       <c r="B21" s="64"/>
       <c r="C21" s="75" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D21" s="67"/>
       <c r="E21" s="72"/>
@@ -4914,7 +4928,7 @@
       <c r="B23" s="64"/>
       <c r="C23" s="72"/>
       <c r="D23" s="59" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E23" s="72" t="s">
         <v>10</v>
@@ -4922,20 +4936,20 @@
       <c r="F23" s="72"/>
       <c r="G23" s="72"/>
       <c r="H23" s="72" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I23" s="80"/>
       <c r="J23" s="72" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="2:10">
       <c r="B24" s="64"/>
       <c r="C24" s="75" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D24" s="67" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E24" s="72"/>
       <c r="F24" s="72"/>
@@ -4959,7 +4973,7 @@
       <c r="B26" s="64"/>
       <c r="C26" s="72"/>
       <c r="D26" s="67" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E26" s="72" t="s">
         <v>10</v>
@@ -4967,20 +4981,20 @@
       <c r="F26" s="72"/>
       <c r="G26" s="72"/>
       <c r="H26" s="72" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I26" s="80"/>
       <c r="J26" s="72" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="2:10">
       <c r="B27" s="64"/>
       <c r="C27" s="75" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D27" s="67" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E27" s="72"/>
       <c r="F27" s="72"/>
@@ -5038,11 +5052,11 @@
     <row r="3" spans="2:15" s="38" customFormat="1">
       <c r="B3" s="139"/>
       <c r="C3" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3" s="24"/>
       <c r="E3" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F3" s="24"/>
       <c r="G3" s="24"/>
@@ -5074,7 +5088,7 @@
     <row r="5" spans="2:15">
       <c r="B5" s="154"/>
       <c r="C5" s="155" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" s="155"/>
       <c r="E5" s="155"/>
@@ -5108,7 +5122,7 @@
     <row r="7" spans="2:15">
       <c r="B7" s="154"/>
       <c r="C7" s="155" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D7" s="155"/>
       <c r="E7" s="155"/>
@@ -5354,7 +5368,7 @@
         <v>1400</v>
       </c>
       <c r="E22" s="155" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F22" s="155"/>
       <c r="G22" s="155"/>
@@ -5434,7 +5448,7 @@
     <row r="27" spans="2:15">
       <c r="B27" s="154"/>
       <c r="C27" s="155" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D27" s="155"/>
       <c r="E27" s="155"/>
@@ -5468,7 +5482,7 @@
     <row r="29" spans="2:15">
       <c r="B29" s="154"/>
       <c r="C29" s="155" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D29" s="155"/>
       <c r="E29" s="155"/>
@@ -5556,7 +5570,7 @@
         <v>4</v>
       </c>
       <c r="E34" s="155" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G34" s="155"/>
       <c r="H34" s="155"/>
@@ -5571,13 +5585,13 @@
     <row r="35" spans="2:15">
       <c r="B35" s="154"/>
       <c r="C35" s="155" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D35" s="155">
         <v>40</v>
       </c>
       <c r="E35" s="155" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G35" s="155"/>
       <c r="H35" s="155"/>
@@ -5786,7 +5800,7 @@
     <row r="48" spans="2:15">
       <c r="B48" s="154"/>
       <c r="C48" s="155" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D48" s="155"/>
       <c r="E48" s="155"/>
@@ -5916,13 +5930,13 @@
     <row r="56" spans="2:15">
       <c r="B56" s="154"/>
       <c r="C56" s="155" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D56" s="159">
         <v>40</v>
       </c>
       <c r="E56" s="159" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F56" s="155"/>
       <c r="G56" s="155"/>
@@ -6002,7 +6016,7 @@
     <row r="61" spans="2:15">
       <c r="B61" s="154"/>
       <c r="C61" s="155" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D61" s="155"/>
       <c r="E61" s="155"/>
@@ -6106,7 +6120,7 @@
         <v>4</v>
       </c>
       <c r="E67" s="155" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G67" s="155"/>
       <c r="H67" s="155"/>

</xml_diff>